<commit_message>
updated report and presentation
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/03b5395bde372c11/Desktop/ETH/8.Semester/Semester Thesis/report/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/03b5395bde372c11/Desktop/ETH/8.Semester/Semester Thesis/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="504" documentId="8_{DE3BA2EC-D09C-4558-8AFB-DBBC027E96C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A93B3478-1DC6-44B7-83D5-4F06D1879A10}"/>
+  <xr:revisionPtr revIDLastSave="565" documentId="8_{DE3BA2EC-D09C-4558-8AFB-DBBC027E96C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A997DC4-30A8-4BBF-82AC-FBC8C1D0757A}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="7395" yWindow="1800" windowWidth="18780" windowHeight="11370" xr2:uid="{2D6B8F3D-09FF-4F02-9B2C-74AB51CD04A8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2D6B8F3D-09FF-4F02-9B2C-74AB51CD04A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcCompleted="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>Model</t>
   </si>
@@ -108,6 +108,33 @@
   </si>
   <si>
     <t>nA</t>
+  </si>
+  <si>
+    <t>CPU</t>
+  </si>
+  <si>
+    <t>GPU</t>
+  </si>
+  <si>
+    <t>DSP</t>
+  </si>
+  <si>
+    <t>HTA</t>
+  </si>
+  <si>
+    <t>fp32</t>
+  </si>
+  <si>
+    <t>int8</t>
+  </si>
+  <si>
+    <t>yolov5n_320</t>
+  </si>
+  <si>
+    <t>yolov5s_320</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -274,7 +301,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -310,6 +337,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1934,7 +1962,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F10968F2-9518-4627-91A8-2E9A6695A0C3}" type="CELLRANGE">
+                    <a:fld id="{B24EC761-0688-4888-9385-CA35C58ADE3F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1974,7 +2002,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{50D159C5-D46D-4041-86A0-84D972F4B76A}" type="CELLRANGE">
+                    <a:fld id="{67A995FD-D0BE-4467-8F8E-96F5BC043637}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2013,7 +2041,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5FE12865-44C5-4532-9249-D27AB24EFDCE}" type="CELLRANGE">
+                    <a:fld id="{A659011A-F338-442F-85C7-6F471F3FCA4B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2052,7 +2080,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5B75A5DD-C58D-4E17-8869-6B1B5A9B36DD}" type="CELLRANGE">
+                    <a:fld id="{7F4E7321-760F-4BEA-8B30-D26D5B3E5F14}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2091,7 +2119,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CA64A408-5B61-43CF-A1A4-D215C8AEC658}" type="CELLRANGE">
+                    <a:fld id="{44939FB7-6DA0-474F-8EAC-42AA3B9D0CA2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2124,7 +2152,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5BDE56C5-67C8-471B-A958-C9F8E61681D6}" type="CELLRANGE">
+                    <a:fld id="{648EAA1F-21E7-43E9-BFA0-5D39899A3A9C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2164,7 +2192,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C0DE8F3E-61EF-4AE6-8B6A-477191636EE0}" type="CELLRANGE">
+                    <a:fld id="{C9326275-67C6-4253-87CB-AECD26F90FFA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2203,7 +2231,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7CEFDADD-AF0C-41C2-891A-A33887A063D3}" type="CELLRANGE">
+                    <a:fld id="{5BE1EEAC-96B5-409A-B912-31FB82F3184A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2242,7 +2270,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5AA428E2-E07D-4E79-997B-D40762A0A80E}" type="CELLRANGE">
+                    <a:fld id="{824688FC-C7A9-461C-AEB9-297B5FA739AB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2281,7 +2309,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4FFFB833-F49E-4A76-8EA1-F01A4075F341}" type="CELLRANGE">
+                    <a:fld id="{27645208-9C05-40C8-8657-6B5AE7AEC285}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2320,7 +2348,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6D217CE1-4B0C-4BAB-A86C-E258997D462B}" type="CELLRANGE">
+                    <a:fld id="{369B29CE-6AF1-4597-AFB7-804FF2F70B1F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2359,7 +2387,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D810B4AE-C4F9-4EE0-8892-42CAA9CDD676}" type="CELLRANGE">
+                    <a:fld id="{28243572-4D3F-4729-BC82-99AA969310EC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2398,7 +2426,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{321AFA91-1C45-466C-AD95-E93454AE69C7}" type="CELLRANGE">
+                    <a:fld id="{2965CEE2-A7AC-49F7-AA64-A34CC18BE952}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2437,7 +2465,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F7939E77-5C5A-48EF-81B5-62089C473415}" type="CELLRANGE">
+                    <a:fld id="{EC9EAFC2-4D1E-4A8D-A7E6-5ED2F4F34FBB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2476,7 +2504,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{93F41B8D-6C42-4D4F-B89F-92A9E863E323}" type="CELLRANGE">
+                    <a:fld id="{9C24347D-8285-49B7-8A29-199309F464CB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5038,6 +5066,1185 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>yolov5n_320</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$83</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>fp32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$81:$E$81</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>CPU</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GPU</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DSP</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>HTA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$83:$E$83</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2DBD-4602-91B1-0465ACD536DF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$84</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>int8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$81:$E$81</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>CPU</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GPU</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DSP</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>HTA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$84:$E$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2DBD-4602-91B1-0465ACD536DF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1842632767"/>
+        <c:axId val="1842642335"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1842632767"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1842642335"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1842642335"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="300"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Inference Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1842632767"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1000">
+          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t>yolov5s_320</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$86</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>fp32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$81:$E$81</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>CPU</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GPU</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DSP</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>HTA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$86:$E$86</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>115</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-33CD-4532-8E0B-6E28A372B011}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$87</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>int8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$81:$E$81</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>CPU</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GPU</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DSP</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>HTA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$87:$E$87</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>61</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-33CD-4532-8E0B-6E28A372B011}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1789860927"/>
+        <c:axId val="1789858431"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1789860927"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1789858431"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1789858431"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Inference Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1789860927"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -5318,6 +6525,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -8352,6 +9639,1012 @@
 </file>
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9234,6 +11527,78 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C251979-F519-9840-860A-BF90C634EE45}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAAC797D-31EB-28EA-B209-22167E9668E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -9534,10 +11899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1447ABD1-59FD-454E-AFC6-2D4274565132}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J75" sqref="J75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9942,6 +12307,104 @@
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F22" s="1"/>
     </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C81" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D81" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E81" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>28</v>
+      </c>
+      <c r="B83">
+        <v>61</v>
+      </c>
+      <c r="C83">
+        <v>170</v>
+      </c>
+      <c r="D83">
+        <v>69</v>
+      </c>
+      <c r="E83">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>29</v>
+      </c>
+      <c r="B84">
+        <v>51</v>
+      </c>
+      <c r="C84">
+        <v>47</v>
+      </c>
+      <c r="D84">
+        <v>18</v>
+      </c>
+      <c r="E84">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>28</v>
+      </c>
+      <c r="B86">
+        <v>124</v>
+      </c>
+      <c r="C86">
+        <v>251</v>
+      </c>
+      <c r="D86">
+        <v>129</v>
+      </c>
+      <c r="E86">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>29</v>
+      </c>
+      <c r="B87">
+        <v>68</v>
+      </c>
+      <c r="C87">
+        <v>62</v>
+      </c>
+      <c r="D87">
+        <v>21</v>
+      </c>
+      <c r="E87">
+        <v>61</v>
+      </c>
+      <c r="F87" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>